<commit_message>
redoing sex bias analyses and cleaning script. Got until halfway H1
</commit_message>
<xml_diff>
--- a/coiba_camtrap_ids_gps.xlsx
+++ b/coiba_camtrap_ids_gps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zoe Goldsborough\Documents\GitHub\camtrap_coiba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51236FDA-E4F5-455A-A805-C25E7FBC1943}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2013CE38-7028-4998-81F6-64FD03C7D61A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1476,8 +1476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="H95" sqref="H95:H142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3927,6 +3927,9 @@
       <c r="G94">
         <v>0</v>
       </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95">
@@ -3976,8 +3979,11 @@
       <c r="G96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>97</v>
       </c>
@@ -3999,8 +4005,11 @@
       <c r="G97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>98</v>
       </c>
@@ -4022,8 +4031,11 @@
       <c r="G98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>99</v>
       </c>
@@ -4045,8 +4057,11 @@
       <c r="G99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>100</v>
       </c>
@@ -4068,8 +4083,11 @@
       <c r="G100">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>101</v>
       </c>
@@ -4091,8 +4109,11 @@
       <c r="G101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>102</v>
       </c>
@@ -4114,8 +4135,11 @@
       <c r="G102">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>103</v>
       </c>
@@ -4137,8 +4161,11 @@
       <c r="G103">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>104</v>
       </c>
@@ -4160,8 +4187,11 @@
       <c r="G104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>105</v>
       </c>
@@ -4183,8 +4213,11 @@
       <c r="G105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>106</v>
       </c>
@@ -4206,8 +4239,11 @@
       <c r="G106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>107</v>
       </c>
@@ -4229,8 +4265,11 @@
       <c r="G107">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>108</v>
       </c>
@@ -4252,8 +4291,11 @@
       <c r="G108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>109</v>
       </c>
@@ -4275,8 +4317,11 @@
       <c r="G109">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>110</v>
       </c>
@@ -4298,8 +4343,11 @@
       <c r="G110">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>111</v>
       </c>
@@ -4321,8 +4369,11 @@
       <c r="G111">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>112</v>
       </c>
@@ -4342,6 +4393,9 @@
         <v>0</v>
       </c>
       <c r="G112">
+        <v>0</v>
+      </c>
+      <c r="H112">
         <v>0</v>
       </c>
     </row>
@@ -4367,6 +4421,9 @@
       <c r="G113">
         <v>0</v>
       </c>
+      <c r="H113">
+        <v>0</v>
+      </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114">
@@ -4390,6 +4447,9 @@
       <c r="G114">
         <v>0</v>
       </c>
+      <c r="H114">
+        <v>0</v>
+      </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115">
@@ -4413,6 +4473,9 @@
       <c r="G115">
         <v>1</v>
       </c>
+      <c r="H115">
+        <v>0</v>
+      </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116">
@@ -4436,6 +4499,9 @@
       <c r="G116">
         <v>1</v>
       </c>
+      <c r="H116">
+        <v>0</v>
+      </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117">
@@ -4459,6 +4525,9 @@
       <c r="G117">
         <v>1</v>
       </c>
+      <c r="H117">
+        <v>0</v>
+      </c>
       <c r="I117" t="s">
         <v>127</v>
       </c>
@@ -4485,6 +4554,9 @@
       <c r="G118">
         <v>1</v>
       </c>
+      <c r="H118">
+        <v>0</v>
+      </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119">
@@ -4508,6 +4580,9 @@
       <c r="G119">
         <v>1</v>
       </c>
+      <c r="H119">
+        <v>0</v>
+      </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120">
@@ -4531,6 +4606,9 @@
       <c r="G120">
         <v>1</v>
       </c>
+      <c r="H120">
+        <v>0</v>
+      </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121">
@@ -4554,6 +4632,9 @@
       <c r="G121">
         <v>1</v>
       </c>
+      <c r="H121">
+        <v>0</v>
+      </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122">
@@ -4577,6 +4658,9 @@
       <c r="G122">
         <v>1</v>
       </c>
+      <c r="H122">
+        <v>0</v>
+      </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123">
@@ -4600,6 +4684,9 @@
       <c r="G123">
         <v>1</v>
       </c>
+      <c r="H123">
+        <v>0</v>
+      </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124">
@@ -4623,6 +4710,9 @@
       <c r="G124">
         <v>1</v>
       </c>
+      <c r="H124">
+        <v>0</v>
+      </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125">
@@ -4646,6 +4736,9 @@
       <c r="G125">
         <v>1</v>
       </c>
+      <c r="H125">
+        <v>0</v>
+      </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126">
@@ -4669,6 +4762,9 @@
       <c r="G126">
         <v>1</v>
       </c>
+      <c r="H126">
+        <v>0</v>
+      </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127">
@@ -4692,6 +4788,9 @@
       <c r="G127">
         <v>1</v>
       </c>
+      <c r="H127">
+        <v>0</v>
+      </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128">
@@ -4715,6 +4814,9 @@
       <c r="G128">
         <v>1</v>
       </c>
+      <c r="H128">
+        <v>0</v>
+      </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129">
@@ -4738,6 +4840,9 @@
       <c r="G129">
         <v>1</v>
       </c>
+      <c r="H129">
+        <v>0</v>
+      </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130">
@@ -4761,6 +4866,9 @@
       <c r="G130">
         <v>1</v>
       </c>
+      <c r="H130">
+        <v>0</v>
+      </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131">
@@ -4784,6 +4892,9 @@
       <c r="G131">
         <v>1</v>
       </c>
+      <c r="H131">
+        <v>0</v>
+      </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132">
@@ -4807,6 +4918,9 @@
       <c r="G132">
         <v>1</v>
       </c>
+      <c r="H132">
+        <v>0</v>
+      </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133">
@@ -4830,6 +4944,9 @@
       <c r="G133">
         <v>1</v>
       </c>
+      <c r="H133">
+        <v>0</v>
+      </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134">
@@ -4853,6 +4970,9 @@
       <c r="G134">
         <v>1</v>
       </c>
+      <c r="H134">
+        <v>0</v>
+      </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135">
@@ -4876,6 +4996,9 @@
       <c r="G135">
         <v>1</v>
       </c>
+      <c r="H135">
+        <v>0</v>
+      </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136">
@@ -4899,6 +5022,9 @@
       <c r="G136">
         <v>1</v>
       </c>
+      <c r="H136">
+        <v>0</v>
+      </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137">
@@ -4949,7 +5075,7 @@
         <v>1</v>
       </c>
       <c r="H138">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.3">
@@ -4973,6 +5099,9 @@
       </c>
       <c r="G139">
         <v>1</v>
+      </c>
+      <c r="H139">
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
cleaning sex bias script , all cams have gps now
</commit_message>
<xml_diff>
--- a/coiba_camtrap_ids_gps.xlsx
+++ b/coiba_camtrap_ids_gps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zoe Goldsborough\Documents\GitHub\camtrap_coiba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2013CE38-7028-4998-81F6-64FD03C7D61A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64E1388-9BDE-40F9-8CC7-AEA9F7EC76AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="210">
   <si>
     <t>number</t>
   </si>
@@ -632,6 +632,24 @@
   </si>
   <si>
     <t>7.2723318</t>
+  </si>
+  <si>
+    <t>J-RAN-12</t>
+  </si>
+  <si>
+    <t>JIC-STREAM-CAMP-NO-T-03</t>
+  </si>
+  <si>
+    <t>-81.8184739</t>
+  </si>
+  <si>
+    <t>7.2680162</t>
+  </si>
+  <si>
+    <t>7.286715</t>
+  </si>
+  <si>
+    <t>-81.802422</t>
   </si>
 </sst>
 </file>
@@ -1474,10 +1492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I142"/>
+  <dimension ref="A1:I144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="H95" sqref="H95:H142"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="H144" sqref="H144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3286,13 +3304,13 @@
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>79</v>
-      </c>
-      <c r="C70" s="1">
-        <v>-81.818305300000006</v>
-      </c>
-      <c r="D70" s="1">
-        <v>7.2662702000000001</v>
+        <v>204</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="E70" t="s">
         <v>9</v>
@@ -3304,7 +3322,7 @@
         <v>1</v>
       </c>
       <c r="H70">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
@@ -3312,13 +3330,13 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C71" s="1">
-        <v>-81.818889100000007</v>
+        <v>-81.818305300000006</v>
       </c>
       <c r="D71" s="1">
-        <v>7.2682161000000001</v>
+        <v>7.2662702000000001</v>
       </c>
       <c r="E71" t="s">
         <v>9</v>
@@ -3338,13 +3356,13 @@
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C72" s="1">
-        <v>-81.819052099999993</v>
+        <v>-81.818889100000007</v>
       </c>
       <c r="D72" s="1">
-        <v>7.2681819000000001</v>
+        <v>7.2682161000000001</v>
       </c>
       <c r="E72" t="s">
         <v>9</v>
@@ -3364,13 +3382,13 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C73" s="1">
-        <v>-81.820685299999994</v>
+        <v>-81.819052099999993</v>
       </c>
       <c r="D73" s="1">
-        <v>7.2708684000000003</v>
+        <v>7.2681819000000001</v>
       </c>
       <c r="E73" t="s">
         <v>9</v>
@@ -3390,13 +3408,13 @@
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C74" s="1">
-        <v>-81.8204645</v>
+        <v>-81.820685299999994</v>
       </c>
       <c r="D74" s="1">
-        <v>7.2710562999999997</v>
+        <v>7.2708684000000003</v>
       </c>
       <c r="E74" t="s">
         <v>9</v>
@@ -3416,13 +3434,13 @@
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C75" s="1">
-        <v>-81.822006799999997</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>202</v>
+        <v>-81.8204645</v>
+      </c>
+      <c r="D75" s="1">
+        <v>7.2710562999999997</v>
       </c>
       <c r="E75" t="s">
         <v>9</v>
@@ -3442,13 +3460,13 @@
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C76" s="1">
-        <v>-81.822063499999999</v>
+        <v>-81.822006799999997</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E76" t="s">
         <v>9</v>
@@ -3468,13 +3486,13 @@
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C77" s="1">
-        <v>-81.821995599999994</v>
-      </c>
-      <c r="D77" s="1">
-        <v>7.2734519000000004</v>
+        <v>-81.822063499999999</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>203</v>
       </c>
       <c r="E77" t="s">
         <v>9</v>
@@ -3494,13 +3512,13 @@
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C78" s="1">
-        <v>-81.820837600000004</v>
+        <v>-81.821995599999994</v>
       </c>
       <c r="D78" s="1">
-        <v>7.2708618999999999</v>
+        <v>7.2734519000000004</v>
       </c>
       <c r="E78" t="s">
         <v>9</v>
@@ -3520,13 +3538,13 @@
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C79" s="1">
-        <v>-81.820339200000006</v>
+        <v>-81.820837600000004</v>
       </c>
       <c r="D79" s="1">
-        <v>7.2711962000000003</v>
+        <v>7.2708618999999999</v>
       </c>
       <c r="E79" t="s">
         <v>9</v>
@@ -3546,13 +3564,13 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C80" s="1">
-        <v>-81.820554799999996</v>
+        <v>-81.820339200000006</v>
       </c>
       <c r="D80" s="1">
-        <v>7.2707516999999999</v>
+        <v>7.2711962000000003</v>
       </c>
       <c r="E80" t="s">
         <v>9</v>
@@ -3572,13 +3590,13 @@
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C81" s="1">
-        <v>-81.818661899999995</v>
+        <v>-81.820554799999996</v>
       </c>
       <c r="D81" s="1">
-        <v>7.2682580999999997</v>
+        <v>7.2707516999999999</v>
       </c>
       <c r="E81" t="s">
         <v>9</v>
@@ -3598,25 +3616,25 @@
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C82" s="1">
-        <v>-81.821717100000001</v>
+        <v>-81.818661899999995</v>
       </c>
       <c r="D82" s="1">
-        <v>7.2718538410000004</v>
+        <v>7.2682580999999997</v>
       </c>
       <c r="E82" t="s">
         <v>9</v>
       </c>
       <c r="F82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G82">
         <v>1</v>
       </c>
       <c r="H82">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
@@ -3624,13 +3642,13 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C83" s="1">
-        <v>-81.820915900000003</v>
+        <v>-81.821717100000001</v>
       </c>
       <c r="D83" s="1">
-        <v>7.2707391000000001</v>
+        <v>7.2718538410000004</v>
       </c>
       <c r="E83" t="s">
         <v>9</v>
@@ -3650,25 +3668,25 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C84" s="1">
-        <v>-81.785812699999994</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>192</v>
+        <v>-81.820915900000003</v>
+      </c>
+      <c r="D84" s="1">
+        <v>7.2707391000000001</v>
       </c>
       <c r="E84" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="F84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G84">
         <v>1</v>
       </c>
       <c r="H84">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
@@ -3676,13 +3694,13 @@
         <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C85" s="1">
-        <v>-81.786137199999999</v>
+        <v>-81.785812699999994</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E85" t="s">
         <v>24</v>
@@ -3702,13 +3720,13 @@
         <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C86" s="1">
-        <v>-81.787318200000001</v>
+        <v>-81.786137199999999</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E86" t="s">
         <v>24</v>
@@ -3728,13 +3746,13 @@
         <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C87" s="1">
-        <v>-81.800081000000006</v>
+        <v>-81.787318200000001</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E87" t="s">
         <v>24</v>
@@ -3754,13 +3772,13 @@
         <v>88</v>
       </c>
       <c r="B88" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C88" s="1">
-        <v>-81.801450000000003</v>
+        <v>-81.800081000000006</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E88" t="s">
         <v>24</v>
@@ -3780,25 +3798,25 @@
         <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C89" s="1">
-        <v>-81.795387240126701</v>
+        <v>-81.801450000000003</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E89" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F89">
         <v>0</v>
       </c>
       <c r="G89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H89">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
@@ -3806,13 +3824,13 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C90" s="1">
-        <v>-81.796470601111594</v>
-      </c>
-      <c r="D90" s="1">
-        <v>7.25505544804036</v>
+        <v>-81.795387240126701</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="E90" t="s">
         <v>9</v>
@@ -3832,13 +3850,13 @@
         <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C91" s="1">
-        <v>-81.795753445476194</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>177</v>
+        <v>-81.796470601111594</v>
+      </c>
+      <c r="D91" s="1">
+        <v>7.25505544804036</v>
       </c>
       <c r="E91" t="s">
         <v>9</v>
@@ -3858,13 +3876,13 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C92" s="1">
-        <v>-81.794891366735101</v>
-      </c>
-      <c r="D92" s="1">
-        <v>7.2541942913085196</v>
+        <v>-81.795753445476194</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="E92" t="s">
         <v>9</v>
@@ -3884,13 +3902,13 @@
         <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C93" s="1">
-        <v>-81.794197093695402</v>
+        <v>-81.794891366735101</v>
       </c>
       <c r="D93" s="1">
-        <v>7.2536945622414297</v>
+        <v>7.2541942913085196</v>
       </c>
       <c r="E93" t="s">
         <v>9</v>
@@ -3910,13 +3928,13 @@
         <v>94</v>
       </c>
       <c r="B94" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C94" s="1">
-        <v>-81.796028120443196</v>
+        <v>-81.794197093695402</v>
       </c>
       <c r="D94" s="1">
-        <v>7.2558889444917396</v>
+        <v>7.2536945622414297</v>
       </c>
       <c r="E94" t="s">
         <v>9</v>
@@ -3936,13 +3954,13 @@
         <v>95</v>
       </c>
       <c r="B95" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C95" s="1">
-        <v>-81.795387240126701</v>
+        <v>-81.796028120443196</v>
       </c>
       <c r="D95" s="1">
-        <v>7.2554998565465203</v>
+        <v>7.2558889444917396</v>
       </c>
       <c r="E95" t="s">
         <v>9</v>
@@ -3962,13 +3980,13 @@
         <v>96</v>
       </c>
       <c r="B96" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C96" s="1">
-        <v>-81.794609064236198</v>
+        <v>-81.795387240126701</v>
       </c>
       <c r="D96" s="1">
-        <v>7.2549443040043098</v>
+        <v>7.2554998565465203</v>
       </c>
       <c r="E96" t="s">
         <v>9</v>
@@ -3988,13 +4006,13 @@
         <v>97</v>
       </c>
       <c r="B97" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C97" s="1">
-        <v>-81.793808005750094</v>
+        <v>-81.794609064236198</v>
       </c>
       <c r="D97" s="1">
-        <v>7.2544998954981503</v>
+        <v>7.2549443040043098</v>
       </c>
       <c r="E97" t="s">
         <v>9</v>
@@ -4014,13 +4032,13 @@
         <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C98" s="1">
-        <v>-81.795608522370401</v>
+        <v>-81.793808005750094</v>
       </c>
       <c r="D98" s="1">
-        <v>7.25658321753144</v>
+        <v>7.2544998954981503</v>
       </c>
       <c r="E98" t="s">
         <v>9</v>
@@ -4040,13 +4058,13 @@
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C99" s="1">
-        <v>-81.794914249330702</v>
+        <v>-81.795608522370401</v>
       </c>
       <c r="D99" s="1">
-        <v>7.2562775295227704</v>
+        <v>7.25658321753144</v>
       </c>
       <c r="E99" t="s">
         <v>9</v>
@@ -4066,13 +4084,13 @@
         <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C100" s="1">
-        <v>-81.794219976291004</v>
+        <v>-81.794914249330702</v>
       </c>
       <c r="D100" s="1">
-        <v>7.2556944005191299</v>
+        <v>7.2562775295227704</v>
       </c>
       <c r="E100" t="s">
         <v>9</v>
@@ -4092,13 +4110,13 @@
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C101" s="1">
-        <v>-81.793281538411904</v>
+        <v>-81.794219976291004</v>
       </c>
       <c r="D101" s="1">
-        <v>7.2553057316690603</v>
+        <v>7.2556944005191299</v>
       </c>
       <c r="E101" t="s">
         <v>9</v>
@@ -4118,13 +4136,13 @@
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C102" s="1">
-        <v>-81.795196551829505</v>
+        <v>-81.793281538411904</v>
       </c>
       <c r="D102" s="1">
-        <v>7.2573333140462601</v>
+        <v>7.2553057316690603</v>
       </c>
       <c r="E102" t="s">
         <v>9</v>
@@ -4144,13 +4162,13 @@
         <v>103</v>
       </c>
       <c r="B103" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C103" s="1">
-        <v>-81.794502278789807</v>
+        <v>-81.795196551829505</v>
       </c>
       <c r="D103" s="1">
-        <v>7.2570557892322496</v>
+        <v>7.2573333140462601</v>
       </c>
       <c r="E103" t="s">
         <v>9</v>
@@ -4170,13 +4188,13 @@
         <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C104" s="1">
-        <v>-81.793609606102095</v>
+        <v>-81.794502278789807</v>
       </c>
       <c r="D104" s="1">
-        <v>7.2564997337758497</v>
+        <v>7.2570557892322496</v>
       </c>
       <c r="E104" t="s">
         <v>9</v>
@@ -4196,13 +4214,13 @@
         <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C105" s="1">
-        <v>-81.792808547616005</v>
+        <v>-81.793609606102095</v>
       </c>
       <c r="D105" s="1">
-        <v>7.2561664693057502</v>
+        <v>7.2564997337758497</v>
       </c>
       <c r="E105" t="s">
         <v>9</v>
@@ -4222,13 +4240,13 @@
         <v>106</v>
       </c>
       <c r="B106" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C106" s="1">
-        <v>-81.7955856397747</v>
+        <v>-81.792808547616005</v>
       </c>
       <c r="D106" s="1">
-        <v>7.2588057629764</v>
+        <v>7.2561664693057502</v>
       </c>
       <c r="E106" t="s">
         <v>9</v>
@@ -4248,13 +4266,13 @@
         <v>107</v>
       </c>
       <c r="B107" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C107" s="1">
-        <v>-81.794670084491301</v>
+        <v>-81.7955856397747</v>
       </c>
       <c r="D107" s="1">
-        <v>7.25827787071466</v>
+        <v>7.2588057629764</v>
       </c>
       <c r="E107" t="s">
         <v>9</v>
@@ -4274,13 +4292,13 @@
         <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C108" s="1">
-        <v>-81.793975811451602</v>
+        <v>-81.794670084491301</v>
       </c>
       <c r="D108" s="1">
-        <v>7.2576942387968302</v>
+        <v>7.25827787071466</v>
       </c>
       <c r="E108" t="s">
         <v>9</v>
@@ -4300,13 +4318,13 @@
         <v>109</v>
       </c>
       <c r="B109" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C109" s="1">
-        <v>-81.793251028284402</v>
+        <v>-81.793975811451602</v>
       </c>
       <c r="D109" s="1">
-        <v>7.2573056537657896</v>
+        <v>7.2576942387968302</v>
       </c>
       <c r="E109" t="s">
         <v>9</v>
@@ -4326,13 +4344,13 @@
         <v>110</v>
       </c>
       <c r="B110" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C110" s="1">
-        <v>-81.792358439415594</v>
+        <v>-81.793251028284402</v>
       </c>
       <c r="D110" s="1">
-        <v>7.2568612452596399</v>
+        <v>7.2573056537657896</v>
       </c>
       <c r="E110" t="s">
         <v>9</v>
@@ -4352,13 +4370,13 @@
         <v>111</v>
       </c>
       <c r="B111" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C111" s="1">
-        <v>-81.792640658095394</v>
+        <v>-81.792358439415594</v>
       </c>
       <c r="D111" s="1">
-        <v>7.2580556664615798</v>
+        <v>7.2568612452596399</v>
       </c>
       <c r="E111" t="s">
         <v>9</v>
@@ -4378,13 +4396,13 @@
         <v>112</v>
       </c>
       <c r="B112" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C112" s="1">
-        <v>-81.791915874928193</v>
+        <v>-81.792640658095394</v>
       </c>
       <c r="D112" s="1">
-        <v>7.2576665785163597</v>
+        <v>7.2580556664615798</v>
       </c>
       <c r="E112" t="s">
         <v>9</v>
@@ -4404,13 +4422,13 @@
         <v>113</v>
       </c>
       <c r="B113" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C113" s="1">
-        <v>-81.791053796187001</v>
+        <v>-81.791915874928193</v>
       </c>
       <c r="D113" s="1">
-        <v>7.2571668494492698</v>
+        <v>7.2576665785163597</v>
       </c>
       <c r="E113" t="s">
         <v>9</v>
@@ -4430,13 +4448,13 @@
         <v>114</v>
       </c>
       <c r="B114" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C114" s="1">
-        <v>-81.790641825646105</v>
+        <v>-81.791053796187001</v>
       </c>
       <c r="D114" s="1">
-        <v>7.2578887827694398</v>
+        <v>7.2571668494492698</v>
       </c>
       <c r="E114" t="s">
         <v>9</v>
@@ -4456,13 +4474,13 @@
         <v>115</v>
       </c>
       <c r="B115" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C115" s="1">
-        <v>-81.822698500000001</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>198</v>
+        <v>-81.790641825646105</v>
+      </c>
+      <c r="D115" s="1">
+        <v>7.2578887827694398</v>
       </c>
       <c r="E115" t="s">
         <v>9</v>
@@ -4471,7 +4489,7 @@
         <v>0</v>
       </c>
       <c r="G115">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H115">
         <v>0</v>
@@ -4482,13 +4500,13 @@
         <v>116</v>
       </c>
       <c r="B116" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C116" s="1">
-        <v>-81.821525534614906</v>
-      </c>
-      <c r="D116" s="1">
-        <v>7.2713331878185201</v>
+        <v>-81.822698500000001</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="E116" t="s">
         <v>9</v>
@@ -4508,13 +4526,13 @@
         <v>117</v>
       </c>
       <c r="B117" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C117" s="1">
-        <v>-81.820335388183494</v>
+        <v>-81.821525534614906</v>
       </c>
       <c r="D117" s="1">
-        <v>7.2699999623000604</v>
+        <v>7.2713331878185201</v>
       </c>
       <c r="E117" t="s">
         <v>9</v>
@@ -4527,9 +4545,6 @@
       </c>
       <c r="H117">
         <v>0</v>
-      </c>
-      <c r="I117" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
@@ -4537,13 +4552,13 @@
         <v>118</v>
       </c>
       <c r="B118" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C118" s="1">
-        <v>-81.819191006943498</v>
+        <v>-81.820335388183494</v>
       </c>
       <c r="D118" s="1">
-        <v>7.2684445325285196</v>
+        <v>7.2699999623000604</v>
       </c>
       <c r="E118" t="s">
         <v>9</v>
@@ -4556,6 +4571,9 @@
       </c>
       <c r="H118">
         <v>0</v>
+      </c>
+      <c r="I118" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
@@ -4563,13 +4581,13 @@
         <v>119</v>
       </c>
       <c r="B119" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C119" s="1">
-        <v>-81.822586096823201</v>
+        <v>-81.819191006943498</v>
       </c>
       <c r="D119" s="1">
-        <v>7.2740001417696396</v>
+        <v>7.2684445325285196</v>
       </c>
       <c r="E119" t="s">
         <v>9</v>
@@ -4589,13 +4607,13 @@
         <v>120</v>
       </c>
       <c r="B120" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C120" s="1">
-        <v>-81.821998609229894</v>
+        <v>-81.822586096823201</v>
       </c>
       <c r="D120" s="1">
-        <v>7.2730279248207799</v>
+        <v>7.2740001417696396</v>
       </c>
       <c r="E120" t="s">
         <v>9</v>
@@ -4615,13 +4633,13 @@
         <v>121</v>
       </c>
       <c r="B121" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C121" s="1">
-        <v>-81.821472141891704</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>178</v>
+        <v>-81.821998609229894</v>
+      </c>
+      <c r="D121" s="1">
+        <v>7.2730279248207799</v>
       </c>
       <c r="E121" t="s">
         <v>9</v>
@@ -4641,13 +4659,13 @@
         <v>122</v>
       </c>
       <c r="B122" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C122" s="1">
-        <v>-81.820754875000006</v>
-      </c>
-      <c r="D122" s="1">
-        <v>7.2715246249999996</v>
+        <v>-81.821472141891704</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="E122" t="s">
         <v>9</v>
@@ -4667,13 +4685,13 @@
         <v>123</v>
       </c>
       <c r="B123" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C123" s="1">
-        <v>-81.820388780906697</v>
+        <v>-81.820754875000006</v>
       </c>
       <c r="D123" s="1">
-        <v>7.2710833232849801</v>
+        <v>7.2715246249999996</v>
       </c>
       <c r="E123" t="s">
         <v>9</v>
@@ -4693,13 +4711,13 @@
         <v>124</v>
       </c>
       <c r="B124" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C124" s="1">
-        <v>-81.819805681666594</v>
+        <v>-81.820388780906697</v>
       </c>
       <c r="D124" s="1">
-        <v>7.2702568950000002</v>
+        <v>7.2710833232849801</v>
       </c>
       <c r="E124" t="s">
         <v>9</v>
@@ -4719,13 +4737,13 @@
         <v>125</v>
       </c>
       <c r="B125" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C125" s="1">
-        <v>-81.819053627550602</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>179</v>
+        <v>-81.819805681666594</v>
+      </c>
+      <c r="D125" s="1">
+        <v>7.2702568950000002</v>
       </c>
       <c r="E125" t="s">
         <v>9</v>
@@ -4745,13 +4763,13 @@
         <v>126</v>
       </c>
       <c r="B126" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C126" s="1">
-        <v>-81.818557754158903</v>
-      </c>
-      <c r="D126" s="1">
-        <v>7.26902774535119</v>
+        <v>-81.819053627550602</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="E126" t="s">
         <v>9</v>
@@ -4771,13 +4789,13 @@
         <v>127</v>
       </c>
       <c r="B127" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C127" s="1">
-        <v>-81.818000776693196</v>
+        <v>-81.818557754158903</v>
       </c>
       <c r="D127" s="1">
-        <v>7.2683058120310298</v>
+        <v>7.26902774535119</v>
       </c>
       <c r="E127" t="s">
         <v>9</v>
@@ -4797,13 +4815,13 @@
         <v>128</v>
       </c>
       <c r="B128" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C128" s="1">
-        <v>-81.821891823783503</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>180</v>
+        <v>-81.818000776693196</v>
+      </c>
+      <c r="D128" s="1">
+        <v>7.2683058120310298</v>
       </c>
       <c r="E128" t="s">
         <v>9</v>
@@ -4823,13 +4841,13 @@
         <v>129</v>
       </c>
       <c r="B129" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C129" s="1">
-        <v>-81.820755000000005</v>
-      </c>
-      <c r="D129" s="1">
-        <v>7.2730119999999996</v>
+        <v>-81.821891823783503</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="E129" t="s">
         <v>9</v>
@@ -4849,13 +4867,13 @@
         <v>130</v>
       </c>
       <c r="B130" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C130" s="1">
-        <v>-81.820165000000003</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>181</v>
+        <v>-81.820755000000005</v>
+      </c>
+      <c r="D130" s="1">
+        <v>7.2730119999999996</v>
       </c>
       <c r="E130" t="s">
         <v>9</v>
@@ -4875,13 +4893,13 @@
         <v>131</v>
       </c>
       <c r="B131" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C131" s="1">
-        <v>-81.819580220000006</v>
-      </c>
-      <c r="D131" s="1">
-        <v>7.2717317750000001</v>
+        <v>-81.820165000000003</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="E131" t="s">
         <v>9</v>
@@ -4901,13 +4919,13 @@
         <v>132</v>
       </c>
       <c r="B132" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C132" s="1">
-        <v>-81.819144508333295</v>
+        <v>-81.819580220000006</v>
       </c>
       <c r="D132" s="1">
-        <v>7.2708083333333304</v>
+        <v>7.2717317750000001</v>
       </c>
       <c r="E132" t="s">
         <v>9</v>
@@ -4927,13 +4945,13 @@
         <v>133</v>
       </c>
       <c r="B133" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C133" s="1">
-        <v>-81.818473851308198</v>
+        <v>-81.819144508333295</v>
       </c>
       <c r="D133" s="1">
-        <v>7.2703333105891899</v>
+        <v>7.2708083333333304</v>
       </c>
       <c r="E133" t="s">
         <v>9</v>
@@ -4953,13 +4971,13 @@
         <v>134</v>
       </c>
       <c r="B134" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C134" s="1">
-        <v>-81.8177795782685</v>
+        <v>-81.818473851308198</v>
       </c>
       <c r="D134" s="1">
-        <v>7.2695555537939001</v>
+        <v>7.2703333105891899</v>
       </c>
       <c r="E134" t="s">
         <v>9</v>
@@ -4979,13 +4997,13 @@
         <v>135</v>
       </c>
       <c r="B135" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C135" s="1">
-        <v>-81.821304336190195</v>
+        <v>-81.8177795782685</v>
       </c>
       <c r="D135" s="1">
-        <v>7.27505542337894</v>
+        <v>7.2695555537939001</v>
       </c>
       <c r="E135" t="s">
         <v>9</v>
@@ -5005,13 +5023,13 @@
         <v>136</v>
       </c>
       <c r="B136" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C136" s="1">
-        <v>-81.820594999999997</v>
+        <v>-81.821304336190195</v>
       </c>
       <c r="D136" s="1">
-        <v>7.2743630000000001</v>
+        <v>7.27505542337894</v>
       </c>
       <c r="E136" t="s">
         <v>9</v>
@@ -5031,13 +5049,13 @@
         <v>137</v>
       </c>
       <c r="B137" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C137" s="1">
-        <v>-81.820030308333301</v>
+        <v>-81.820594999999997</v>
       </c>
       <c r="D137" s="1">
-        <v>7.2736376766666604</v>
+        <v>7.2743630000000001</v>
       </c>
       <c r="E137" t="s">
         <v>9</v>
@@ -5057,13 +5075,13 @@
         <v>138</v>
       </c>
       <c r="B138" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C138" s="1">
-        <v>-81.819337298333295</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>182</v>
+        <v>-81.820030308333301</v>
+      </c>
+      <c r="D138" s="1">
+        <v>7.2736376766666604</v>
       </c>
       <c r="E138" t="s">
         <v>9</v>
@@ -5083,13 +5101,13 @@
         <v>139</v>
       </c>
       <c r="B139" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C139" s="1">
-        <v>-81.818996999999996</v>
+        <v>-81.819337298333295</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E139" t="s">
         <v>9</v>
@@ -5109,13 +5127,13 @@
         <v>140</v>
       </c>
       <c r="B140" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C140" s="1">
-        <v>-81.818292045000007</v>
-      </c>
-      <c r="D140" s="1">
-        <v>7.2714530616666604</v>
+        <v>-81.818996999999996</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="E140" t="s">
         <v>9</v>
@@ -5135,13 +5153,13 @@
         <v>141</v>
       </c>
       <c r="B141" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C141" s="1">
-        <v>-81.817802460864101</v>
+        <v>-81.818292045000007</v>
       </c>
       <c r="D141" s="1">
-        <v>7.2707500588148797</v>
+        <v>7.2714530616666604</v>
       </c>
       <c r="E141" t="s">
         <v>9</v>
@@ -5161,28 +5179,81 @@
         <v>142</v>
       </c>
       <c r="B142" t="s">
+        <v>151</v>
+      </c>
+      <c r="C142" s="1">
+        <v>-81.817802460864101</v>
+      </c>
+      <c r="D142" s="1">
+        <v>7.2707500588148797</v>
+      </c>
+      <c r="E142" t="s">
+        <v>9</v>
+      </c>
+      <c r="F142">
+        <v>0</v>
+      </c>
+      <c r="G142">
+        <v>1</v>
+      </c>
+      <c r="H142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <v>143</v>
+      </c>
+      <c r="B143" t="s">
         <v>152</v>
       </c>
-      <c r="C142" s="1">
+      <c r="C143" s="1">
         <v>-81.816581720486198</v>
       </c>
-      <c r="D142" s="1">
+      <c r="D143" s="1">
         <v>7.26930568926036</v>
       </c>
-      <c r="E142" t="s">
-        <v>9</v>
-      </c>
-      <c r="F142">
-        <v>0</v>
-      </c>
-      <c r="G142">
-        <v>1</v>
-      </c>
-      <c r="H142">
-        <v>0</v>
+      <c r="E143" t="s">
+        <v>9</v>
+      </c>
+      <c r="F143">
+        <v>0</v>
+      </c>
+      <c r="G143">
+        <v>1</v>
+      </c>
+      <c r="H143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>144</v>
+      </c>
+      <c r="B144" t="s">
+        <v>205</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E144" t="s">
+        <v>9</v>
+      </c>
+      <c r="F144">
+        <v>0</v>
+      </c>
+      <c r="G144">
+        <v>0</v>
+      </c>
+      <c r="H144">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dealt with identifying pick/set up days accurately, re-did sex bias analyses
</commit_message>
<xml_diff>
--- a/coiba_camtrap_ids_gps.xlsx
+++ b/coiba_camtrap_ids_gps.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zoe Goldsborough\Documents\GitHub\camtrap_coiba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64E1388-9BDE-40F9-8CC7-AEA9F7EC76AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD679F8A-ECAC-4197-A65E-D78AD8AF40E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="217">
   <si>
     <t>number</t>
   </si>
@@ -650,6 +650,27 @@
   </si>
   <si>
     <t>-81.802422</t>
+  </si>
+  <si>
+    <t>side</t>
+  </si>
+  <si>
+    <t>west</t>
+  </si>
+  <si>
+    <t>north</t>
+  </si>
+  <si>
+    <t>east</t>
+  </si>
+  <si>
+    <t>southeast</t>
+  </si>
+  <si>
+    <t>south</t>
+  </si>
+  <si>
+    <t>northwest</t>
   </si>
 </sst>
 </file>
@@ -1492,10 +1513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I144"/>
+  <dimension ref="A1:J144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="H144" sqref="H144"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1505,7 +1526,7 @@
     <col min="4" max="4" width="42.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1522,16 +1543,19 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1547,8 +1571,8 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F2">
-        <v>0</v>
+      <c r="F2" t="s">
+        <v>212</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -1556,8 +1580,11 @@
       <c r="H2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1573,8 +1600,8 @@
       <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="F3">
-        <v>0</v>
+      <c r="F3" t="s">
+        <v>214</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -1582,8 +1609,11 @@
       <c r="H3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1599,8 +1629,8 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="F4">
-        <v>0</v>
+      <c r="F4" t="s">
+        <v>214</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -1608,8 +1638,11 @@
       <c r="H4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1625,8 +1658,8 @@
       <c r="E5" t="s">
         <v>9</v>
       </c>
-      <c r="F5">
-        <v>0</v>
+      <c r="F5" t="s">
+        <v>215</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1634,8 +1667,11 @@
       <c r="H5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1651,8 +1687,8 @@
       <c r="E6" t="s">
         <v>9</v>
       </c>
-      <c r="F6">
-        <v>0</v>
+      <c r="F6" t="s">
+        <v>215</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1660,8 +1696,11 @@
       <c r="H6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1677,8 +1716,8 @@
       <c r="E7" t="s">
         <v>9</v>
       </c>
-      <c r="F7">
-        <v>0</v>
+      <c r="F7" t="s">
+        <v>215</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1686,8 +1725,11 @@
       <c r="H7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1703,8 +1745,8 @@
       <c r="E8" t="s">
         <v>9</v>
       </c>
-      <c r="F8">
-        <v>0</v>
+      <c r="F8" t="s">
+        <v>212</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1712,8 +1754,11 @@
       <c r="H8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1729,8 +1774,8 @@
       <c r="E9" t="s">
         <v>9</v>
       </c>
-      <c r="F9">
-        <v>0</v>
+      <c r="F9" t="s">
+        <v>215</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1738,8 +1783,11 @@
       <c r="H9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1755,17 +1803,20 @@
       <c r="E10" t="s">
         <v>9</v>
       </c>
-      <c r="F10">
-        <v>1</v>
+      <c r="F10" t="s">
+        <v>211</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1781,17 +1832,20 @@
       <c r="E11" t="s">
         <v>9</v>
       </c>
-      <c r="F11">
-        <v>1</v>
+      <c r="F11" t="s">
+        <v>211</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1807,17 +1861,20 @@
       <c r="E12" t="s">
         <v>9</v>
       </c>
-      <c r="F12">
-        <v>0</v>
+      <c r="F12" t="s">
+        <v>211</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1833,8 +1890,8 @@
       <c r="E13" t="s">
         <v>9</v>
       </c>
-      <c r="F13">
-        <v>0</v>
+      <c r="F13" t="s">
+        <v>213</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -1842,8 +1899,11 @@
       <c r="H13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1859,8 +1919,8 @@
       <c r="E14" t="s">
         <v>9</v>
       </c>
-      <c r="F14">
-        <v>0</v>
+      <c r="F14" t="s">
+        <v>213</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1868,8 +1928,11 @@
       <c r="H14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1885,8 +1948,8 @@
       <c r="E15" t="s">
         <v>9</v>
       </c>
-      <c r="F15">
-        <v>0</v>
+      <c r="F15" t="s">
+        <v>212</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1894,8 +1957,11 @@
       <c r="H15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1911,8 +1977,8 @@
       <c r="E16" t="s">
         <v>24</v>
       </c>
-      <c r="F16">
-        <v>0</v>
+      <c r="F16" t="s">
+        <v>213</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -1920,8 +1986,11 @@
       <c r="H16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1937,8 +2006,8 @@
       <c r="E17" t="s">
         <v>24</v>
       </c>
-      <c r="F17">
-        <v>0</v>
+      <c r="F17" t="s">
+        <v>213</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1946,8 +2015,11 @@
       <c r="H17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1963,8 +2035,8 @@
       <c r="E18" t="s">
         <v>9</v>
       </c>
-      <c r="F18">
-        <v>0</v>
+      <c r="F18" t="s">
+        <v>215</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -1972,8 +2044,11 @@
       <c r="H18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1989,8 +2064,8 @@
       <c r="E19" t="s">
         <v>9</v>
       </c>
-      <c r="F19">
-        <v>0</v>
+      <c r="F19" t="s">
+        <v>215</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -1998,8 +2073,11 @@
       <c r="H19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2015,8 +2093,8 @@
       <c r="E20" t="s">
         <v>24</v>
       </c>
-      <c r="F20">
-        <v>0</v>
+      <c r="F20" t="s">
+        <v>216</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -2024,8 +2102,11 @@
       <c r="H20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2041,8 +2122,8 @@
       <c r="E21" t="s">
         <v>24</v>
       </c>
-      <c r="F21">
-        <v>0</v>
+      <c r="F21" t="s">
+        <v>216</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -2050,8 +2131,11 @@
       <c r="H21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2067,17 +2151,20 @@
       <c r="E22" t="s">
         <v>9</v>
       </c>
-      <c r="F22">
-        <v>0</v>
+      <c r="F22" t="s">
+        <v>211</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2093,17 +2180,20 @@
       <c r="E23" t="s">
         <v>9</v>
       </c>
-      <c r="F23">
-        <v>0</v>
+      <c r="F23" t="s">
+        <v>211</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2119,17 +2209,20 @@
       <c r="E24" t="s">
         <v>9</v>
       </c>
-      <c r="F24">
-        <v>1</v>
+      <c r="F24" t="s">
+        <v>211</v>
       </c>
       <c r="G24">
         <v>1</v>
       </c>
       <c r="H24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2145,17 +2238,20 @@
       <c r="E25" t="s">
         <v>9</v>
       </c>
-      <c r="F25">
-        <v>1</v>
+      <c r="F25" t="s">
+        <v>211</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
       <c r="H25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2171,8 +2267,8 @@
       <c r="E26" t="s">
         <v>9</v>
       </c>
-      <c r="F26">
-        <v>1</v>
+      <c r="F26" t="s">
+        <v>211</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -2180,8 +2276,11 @@
       <c r="H26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2197,17 +2296,20 @@
       <c r="E27" t="s">
         <v>9</v>
       </c>
-      <c r="F27">
-        <v>1</v>
+      <c r="F27" t="s">
+        <v>211</v>
       </c>
       <c r="G27">
         <v>1</v>
       </c>
       <c r="H27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2223,8 +2325,8 @@
       <c r="E28" t="s">
         <v>9</v>
       </c>
-      <c r="F28">
-        <v>0</v>
+      <c r="F28" t="s">
+        <v>213</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -2232,8 +2334,11 @@
       <c r="H28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2249,8 +2354,8 @@
       <c r="E29" t="s">
         <v>9</v>
       </c>
-      <c r="F29">
-        <v>0</v>
+      <c r="F29" t="s">
+        <v>212</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -2258,8 +2363,11 @@
       <c r="H29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2275,8 +2383,8 @@
       <c r="E30" t="s">
         <v>9</v>
       </c>
-      <c r="F30">
-        <v>0</v>
+      <c r="F30" t="s">
+        <v>212</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -2284,8 +2392,11 @@
       <c r="H30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2301,17 +2412,17 @@
       <c r="E31" t="s">
         <v>40</v>
       </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
       <c r="G31">
         <v>0</v>
       </c>
       <c r="H31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2327,8 +2438,8 @@
       <c r="E32" t="s">
         <v>9</v>
       </c>
-      <c r="F32">
-        <v>0</v>
+      <c r="F32" t="s">
+        <v>215</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -2336,8 +2447,11 @@
       <c r="H32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2353,17 +2467,20 @@
       <c r="E33" t="s">
         <v>9</v>
       </c>
-      <c r="F33">
-        <v>1</v>
+      <c r="F33" t="s">
+        <v>211</v>
       </c>
       <c r="G33">
         <v>1</v>
       </c>
       <c r="H33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2379,17 +2496,20 @@
       <c r="E34" t="s">
         <v>9</v>
       </c>
-      <c r="F34">
-        <v>0</v>
+      <c r="F34" t="s">
+        <v>211</v>
       </c>
       <c r="G34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2405,17 +2525,20 @@
       <c r="E35" t="s">
         <v>9</v>
       </c>
-      <c r="F35">
-        <v>1</v>
+      <c r="F35" t="s">
+        <v>211</v>
       </c>
       <c r="G35">
         <v>1</v>
       </c>
       <c r="H35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2431,8 +2554,8 @@
       <c r="E36" t="s">
         <v>9</v>
       </c>
-      <c r="F36">
-        <v>1</v>
+      <c r="F36" t="s">
+        <v>211</v>
       </c>
       <c r="G36">
         <v>1</v>
@@ -2440,8 +2563,11 @@
       <c r="H36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2457,8 +2583,8 @@
       <c r="E37" t="s">
         <v>9</v>
       </c>
-      <c r="F37">
-        <v>0</v>
+      <c r="F37" t="s">
+        <v>214</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -2466,8 +2592,11 @@
       <c r="H37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2483,8 +2612,8 @@
       <c r="E38" t="s">
         <v>9</v>
       </c>
-      <c r="F38">
-        <v>0</v>
+      <c r="F38" t="s">
+        <v>212</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -2492,8 +2621,11 @@
       <c r="H38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2509,8 +2641,8 @@
       <c r="E39" t="s">
         <v>9</v>
       </c>
-      <c r="F39">
-        <v>0</v>
+      <c r="F39" t="s">
+        <v>212</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -2518,8 +2650,11 @@
       <c r="H39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2535,17 +2670,20 @@
       <c r="E40" t="s">
         <v>9</v>
       </c>
-      <c r="F40">
-        <v>1</v>
+      <c r="F40" t="s">
+        <v>211</v>
       </c>
       <c r="G40">
         <v>1</v>
       </c>
       <c r="H40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2561,17 +2699,20 @@
       <c r="E41" t="s">
         <v>9</v>
       </c>
-      <c r="F41">
-        <v>0</v>
+      <c r="F41" t="s">
+        <v>211</v>
       </c>
       <c r="G41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2587,17 +2728,20 @@
       <c r="E42" t="s">
         <v>9</v>
       </c>
-      <c r="F42">
-        <v>1</v>
+      <c r="F42" t="s">
+        <v>211</v>
       </c>
       <c r="G42">
         <v>1</v>
       </c>
       <c r="H42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2613,8 +2757,8 @@
       <c r="E43" t="s">
         <v>9</v>
       </c>
-      <c r="F43">
-        <v>1</v>
+      <c r="F43" t="s">
+        <v>211</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -2622,8 +2766,11 @@
       <c r="H43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2639,8 +2786,8 @@
       <c r="E44" t="s">
         <v>9</v>
       </c>
-      <c r="F44">
-        <v>0</v>
+      <c r="F44" t="s">
+        <v>212</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -2648,8 +2795,11 @@
       <c r="H44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2665,17 +2815,20 @@
       <c r="E45" t="s">
         <v>9</v>
       </c>
-      <c r="F45">
-        <v>1</v>
+      <c r="F45" t="s">
+        <v>211</v>
       </c>
       <c r="G45">
         <v>1</v>
       </c>
       <c r="H45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2691,8 +2844,8 @@
       <c r="E46" t="s">
         <v>9</v>
       </c>
-      <c r="F46">
-        <v>1</v>
+      <c r="F46" t="s">
+        <v>211</v>
       </c>
       <c r="G46">
         <v>1</v>
@@ -2700,8 +2853,11 @@
       <c r="H46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2717,17 +2873,20 @@
       <c r="E47" t="s">
         <v>9</v>
       </c>
-      <c r="F47">
-        <v>0</v>
+      <c r="F47" t="s">
+        <v>212</v>
       </c>
       <c r="G47">
         <v>0</v>
       </c>
       <c r="H47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2743,17 +2902,20 @@
       <c r="E48" t="s">
         <v>9</v>
       </c>
-      <c r="F48">
-        <v>0</v>
+      <c r="F48" t="s">
+        <v>212</v>
       </c>
       <c r="G48">
         <v>0</v>
       </c>
       <c r="H48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>49</v>
       </c>
@@ -2769,17 +2931,20 @@
       <c r="E49" t="s">
         <v>9</v>
       </c>
-      <c r="F49">
-        <v>0</v>
+      <c r="F49" t="s">
+        <v>211</v>
       </c>
       <c r="G49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>50</v>
       </c>
@@ -2795,17 +2960,20 @@
       <c r="E50" t="s">
         <v>9</v>
       </c>
-      <c r="F50">
-        <v>0</v>
+      <c r="F50" t="s">
+        <v>211</v>
       </c>
       <c r="G50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>51</v>
       </c>
@@ -2821,17 +2989,20 @@
       <c r="E51" t="s">
         <v>9</v>
       </c>
-      <c r="F51">
-        <v>0</v>
+      <c r="F51" t="s">
+        <v>211</v>
       </c>
       <c r="G51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>52</v>
       </c>
@@ -2847,17 +3018,20 @@
       <c r="E52" t="s">
         <v>9</v>
       </c>
-      <c r="F52">
-        <v>1</v>
+      <c r="F52" t="s">
+        <v>211</v>
       </c>
       <c r="G52">
         <v>1</v>
       </c>
       <c r="H52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>53</v>
       </c>
@@ -2873,17 +3047,20 @@
       <c r="E53" t="s">
         <v>24</v>
       </c>
-      <c r="F53">
-        <v>0</v>
+      <c r="F53" t="s">
+        <v>216</v>
       </c>
       <c r="G53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>54</v>
       </c>
@@ -2899,17 +3076,20 @@
       <c r="E54" t="s">
         <v>24</v>
       </c>
-      <c r="F54">
-        <v>0</v>
+      <c r="F54" t="s">
+        <v>216</v>
       </c>
       <c r="G54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>55</v>
       </c>
@@ -2925,17 +3105,20 @@
       <c r="E55" t="s">
         <v>24</v>
       </c>
-      <c r="F55">
-        <v>0</v>
+      <c r="F55" t="s">
+        <v>216</v>
       </c>
       <c r="G55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>56</v>
       </c>
@@ -2951,17 +3134,20 @@
       <c r="E56" t="s">
         <v>24</v>
       </c>
-      <c r="F56">
-        <v>0</v>
+      <c r="F56" t="s">
+        <v>216</v>
       </c>
       <c r="G56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>57</v>
       </c>
@@ -2977,17 +3163,20 @@
       <c r="E57" t="s">
         <v>9</v>
       </c>
-      <c r="F57">
-        <v>1</v>
+      <c r="F57" t="s">
+        <v>211</v>
       </c>
       <c r="G57">
         <v>1</v>
       </c>
       <c r="H57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>58</v>
       </c>
@@ -3003,17 +3192,20 @@
       <c r="E58" t="s">
         <v>9</v>
       </c>
-      <c r="F58">
-        <v>1</v>
+      <c r="F58" t="s">
+        <v>211</v>
       </c>
       <c r="G58">
         <v>1</v>
       </c>
       <c r="H58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>59</v>
       </c>
@@ -3029,17 +3221,20 @@
       <c r="E59" t="s">
         <v>9</v>
       </c>
-      <c r="F59">
-        <v>0</v>
+      <c r="F59" t="s">
+        <v>211</v>
       </c>
       <c r="G59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>60</v>
       </c>
@@ -3055,17 +3250,20 @@
       <c r="E60" t="s">
         <v>9</v>
       </c>
-      <c r="F60">
-        <v>0</v>
+      <c r="F60" t="s">
+        <v>211</v>
       </c>
       <c r="G60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>61</v>
       </c>
@@ -3081,17 +3279,20 @@
       <c r="E61" t="s">
         <v>9</v>
       </c>
-      <c r="F61">
-        <v>0</v>
+      <c r="F61" t="s">
+        <v>211</v>
       </c>
       <c r="G61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>62</v>
       </c>
@@ -3107,17 +3308,20 @@
       <c r="E62" t="s">
         <v>9</v>
       </c>
-      <c r="F62">
-        <v>0</v>
+      <c r="F62" t="s">
+        <v>211</v>
       </c>
       <c r="G62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>63</v>
       </c>
@@ -3133,17 +3337,20 @@
       <c r="E63" t="s">
         <v>9</v>
       </c>
-      <c r="F63">
-        <v>0</v>
+      <c r="F63" t="s">
+        <v>211</v>
       </c>
       <c r="G63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>64</v>
       </c>
@@ -3159,17 +3366,20 @@
       <c r="E64" t="s">
         <v>9</v>
       </c>
-      <c r="F64">
-        <v>0</v>
+      <c r="F64" t="s">
+        <v>211</v>
       </c>
       <c r="G64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>65</v>
       </c>
@@ -3185,17 +3395,20 @@
       <c r="E65" t="s">
         <v>9</v>
       </c>
-      <c r="F65">
-        <v>0</v>
+      <c r="F65" t="s">
+        <v>211</v>
       </c>
       <c r="G65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>66</v>
       </c>
@@ -3211,17 +3424,20 @@
       <c r="E66" t="s">
         <v>9</v>
       </c>
-      <c r="F66">
-        <v>0</v>
+      <c r="F66" t="s">
+        <v>211</v>
       </c>
       <c r="G66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>67</v>
       </c>
@@ -3237,17 +3453,20 @@
       <c r="E67" t="s">
         <v>9</v>
       </c>
-      <c r="F67">
-        <v>0</v>
+      <c r="F67" t="s">
+        <v>211</v>
       </c>
       <c r="G67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>68</v>
       </c>
@@ -3263,17 +3482,20 @@
       <c r="E68" t="s">
         <v>9</v>
       </c>
-      <c r="F68">
-        <v>0</v>
+      <c r="F68" t="s">
+        <v>211</v>
       </c>
       <c r="G68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>69</v>
       </c>
@@ -3289,17 +3511,20 @@
       <c r="E69" t="s">
         <v>9</v>
       </c>
-      <c r="F69">
-        <v>0</v>
+      <c r="F69" t="s">
+        <v>211</v>
       </c>
       <c r="G69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>70</v>
       </c>
@@ -3315,17 +3540,20 @@
       <c r="E70" t="s">
         <v>9</v>
       </c>
-      <c r="F70">
-        <v>0</v>
+      <c r="F70" t="s">
+        <v>211</v>
       </c>
       <c r="G70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>71</v>
       </c>
@@ -3341,17 +3569,20 @@
       <c r="E71" t="s">
         <v>9</v>
       </c>
-      <c r="F71">
-        <v>0</v>
+      <c r="F71" t="s">
+        <v>211</v>
       </c>
       <c r="G71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>72</v>
       </c>
@@ -3367,17 +3598,20 @@
       <c r="E72" t="s">
         <v>9</v>
       </c>
-      <c r="F72">
-        <v>0</v>
+      <c r="F72" t="s">
+        <v>211</v>
       </c>
       <c r="G72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H72">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>73</v>
       </c>
@@ -3393,17 +3627,20 @@
       <c r="E73" t="s">
         <v>9</v>
       </c>
-      <c r="F73">
-        <v>0</v>
+      <c r="F73" t="s">
+        <v>211</v>
       </c>
       <c r="G73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>74</v>
       </c>
@@ -3419,17 +3656,20 @@
       <c r="E74" t="s">
         <v>9</v>
       </c>
-      <c r="F74">
-        <v>0</v>
+      <c r="F74" t="s">
+        <v>211</v>
       </c>
       <c r="G74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>75</v>
       </c>
@@ -3445,17 +3685,20 @@
       <c r="E75" t="s">
         <v>9</v>
       </c>
-      <c r="F75">
-        <v>0</v>
+      <c r="F75" t="s">
+        <v>211</v>
       </c>
       <c r="G75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>76</v>
       </c>
@@ -3471,17 +3714,20 @@
       <c r="E76" t="s">
         <v>9</v>
       </c>
-      <c r="F76">
-        <v>0</v>
+      <c r="F76" t="s">
+        <v>211</v>
       </c>
       <c r="G76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>77</v>
       </c>
@@ -3497,17 +3743,20 @@
       <c r="E77" t="s">
         <v>9</v>
       </c>
-      <c r="F77">
-        <v>0</v>
+      <c r="F77" t="s">
+        <v>211</v>
       </c>
       <c r="G77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H77">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>78</v>
       </c>
@@ -3523,17 +3772,20 @@
       <c r="E78" t="s">
         <v>9</v>
       </c>
-      <c r="F78">
-        <v>0</v>
+      <c r="F78" t="s">
+        <v>211</v>
       </c>
       <c r="G78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H78">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>79</v>
       </c>
@@ -3549,17 +3801,20 @@
       <c r="E79" t="s">
         <v>9</v>
       </c>
-      <c r="F79">
-        <v>0</v>
+      <c r="F79" t="s">
+        <v>211</v>
       </c>
       <c r="G79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H79">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>80</v>
       </c>
@@ -3575,17 +3830,20 @@
       <c r="E80" t="s">
         <v>9</v>
       </c>
-      <c r="F80">
-        <v>0</v>
+      <c r="F80" t="s">
+        <v>211</v>
       </c>
       <c r="G80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>81</v>
       </c>
@@ -3601,17 +3859,20 @@
       <c r="E81" t="s">
         <v>9</v>
       </c>
-      <c r="F81">
-        <v>0</v>
+      <c r="F81" t="s">
+        <v>211</v>
       </c>
       <c r="G81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H81">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>82</v>
       </c>
@@ -3627,17 +3888,20 @@
       <c r="E82" t="s">
         <v>9</v>
       </c>
-      <c r="F82">
-        <v>0</v>
+      <c r="F82" t="s">
+        <v>211</v>
       </c>
       <c r="G82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H82">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>83</v>
       </c>
@@ -3653,17 +3917,20 @@
       <c r="E83" t="s">
         <v>9</v>
       </c>
-      <c r="F83">
-        <v>1</v>
+      <c r="F83" t="s">
+        <v>211</v>
       </c>
       <c r="G83">
         <v>1</v>
       </c>
       <c r="H83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>84</v>
       </c>
@@ -3679,17 +3946,20 @@
       <c r="E84" t="s">
         <v>9</v>
       </c>
-      <c r="F84">
-        <v>1</v>
+      <c r="F84" t="s">
+        <v>211</v>
       </c>
       <c r="G84">
         <v>1</v>
       </c>
       <c r="H84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>85</v>
       </c>
@@ -3705,17 +3975,20 @@
       <c r="E85" t="s">
         <v>24</v>
       </c>
-      <c r="F85">
-        <v>0</v>
+      <c r="F85" t="s">
+        <v>216</v>
       </c>
       <c r="G85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H85">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>86</v>
       </c>
@@ -3731,17 +4004,20 @@
       <c r="E86" t="s">
         <v>24</v>
       </c>
-      <c r="F86">
-        <v>0</v>
+      <c r="F86" t="s">
+        <v>216</v>
       </c>
       <c r="G86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H86">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>87</v>
       </c>
@@ -3757,17 +4033,20 @@
       <c r="E87" t="s">
         <v>24</v>
       </c>
-      <c r="F87">
-        <v>0</v>
+      <c r="F87" t="s">
+        <v>216</v>
       </c>
       <c r="G87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H87">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>88</v>
       </c>
@@ -3783,17 +4062,20 @@
       <c r="E88" t="s">
         <v>24</v>
       </c>
-      <c r="F88">
-        <v>0</v>
+      <c r="F88" t="s">
+        <v>216</v>
       </c>
       <c r="G88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H88">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>89</v>
       </c>
@@ -3809,17 +4091,20 @@
       <c r="E89" t="s">
         <v>24</v>
       </c>
-      <c r="F89">
-        <v>0</v>
+      <c r="F89" t="s">
+        <v>216</v>
       </c>
       <c r="G89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H89">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>90</v>
       </c>
@@ -3835,8 +4120,8 @@
       <c r="E90" t="s">
         <v>9</v>
       </c>
-      <c r="F90">
-        <v>0</v>
+      <c r="F90" t="s">
+        <v>213</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -3844,8 +4129,11 @@
       <c r="H90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>91</v>
       </c>
@@ -3861,8 +4149,8 @@
       <c r="E91" t="s">
         <v>9</v>
       </c>
-      <c r="F91">
-        <v>0</v>
+      <c r="F91" t="s">
+        <v>213</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -3870,8 +4158,11 @@
       <c r="H91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>92</v>
       </c>
@@ -3887,8 +4178,8 @@
       <c r="E92" t="s">
         <v>9</v>
       </c>
-      <c r="F92">
-        <v>0</v>
+      <c r="F92" t="s">
+        <v>213</v>
       </c>
       <c r="G92">
         <v>0</v>
@@ -3896,8 +4187,11 @@
       <c r="H92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>93</v>
       </c>
@@ -3913,8 +4207,8 @@
       <c r="E93" t="s">
         <v>9</v>
       </c>
-      <c r="F93">
-        <v>0</v>
+      <c r="F93" t="s">
+        <v>213</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -3922,8 +4216,11 @@
       <c r="H93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>94</v>
       </c>
@@ -3939,8 +4236,8 @@
       <c r="E94" t="s">
         <v>9</v>
       </c>
-      <c r="F94">
-        <v>0</v>
+      <c r="F94" t="s">
+        <v>213</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -3948,8 +4245,11 @@
       <c r="H94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>95</v>
       </c>
@@ -3965,8 +4265,8 @@
       <c r="E95" t="s">
         <v>9</v>
       </c>
-      <c r="F95">
-        <v>0</v>
+      <c r="F95" t="s">
+        <v>213</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -3974,8 +4274,11 @@
       <c r="H95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>96</v>
       </c>
@@ -3991,8 +4294,8 @@
       <c r="E96" t="s">
         <v>9</v>
       </c>
-      <c r="F96">
-        <v>0</v>
+      <c r="F96" t="s">
+        <v>213</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -4000,8 +4303,11 @@
       <c r="H96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>97</v>
       </c>
@@ -4017,8 +4323,8 @@
       <c r="E97" t="s">
         <v>9</v>
       </c>
-      <c r="F97">
-        <v>0</v>
+      <c r="F97" t="s">
+        <v>213</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -4026,8 +4332,11 @@
       <c r="H97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>98</v>
       </c>
@@ -4043,8 +4352,8 @@
       <c r="E98" t="s">
         <v>9</v>
       </c>
-      <c r="F98">
-        <v>0</v>
+      <c r="F98" t="s">
+        <v>213</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -4052,8 +4361,11 @@
       <c r="H98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>99</v>
       </c>
@@ -4069,8 +4381,8 @@
       <c r="E99" t="s">
         <v>9</v>
       </c>
-      <c r="F99">
-        <v>0</v>
+      <c r="F99" t="s">
+        <v>213</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -4078,8 +4390,11 @@
       <c r="H99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>100</v>
       </c>
@@ -4095,8 +4410,8 @@
       <c r="E100" t="s">
         <v>9</v>
       </c>
-      <c r="F100">
-        <v>0</v>
+      <c r="F100" t="s">
+        <v>213</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -4104,8 +4419,11 @@
       <c r="H100">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>101</v>
       </c>
@@ -4121,8 +4439,8 @@
       <c r="E101" t="s">
         <v>9</v>
       </c>
-      <c r="F101">
-        <v>0</v>
+      <c r="F101" t="s">
+        <v>213</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -4130,8 +4448,11 @@
       <c r="H101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>102</v>
       </c>
@@ -4147,8 +4468,8 @@
       <c r="E102" t="s">
         <v>9</v>
       </c>
-      <c r="F102">
-        <v>0</v>
+      <c r="F102" t="s">
+        <v>213</v>
       </c>
       <c r="G102">
         <v>0</v>
@@ -4156,8 +4477,11 @@
       <c r="H102">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>103</v>
       </c>
@@ -4173,8 +4497,8 @@
       <c r="E103" t="s">
         <v>9</v>
       </c>
-      <c r="F103">
-        <v>0</v>
+      <c r="F103" t="s">
+        <v>213</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -4182,8 +4506,11 @@
       <c r="H103">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>104</v>
       </c>
@@ -4199,8 +4526,8 @@
       <c r="E104" t="s">
         <v>9</v>
       </c>
-      <c r="F104">
-        <v>0</v>
+      <c r="F104" t="s">
+        <v>213</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -4208,8 +4535,11 @@
       <c r="H104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>105</v>
       </c>
@@ -4225,8 +4555,8 @@
       <c r="E105" t="s">
         <v>9</v>
       </c>
-      <c r="F105">
-        <v>0</v>
+      <c r="F105" t="s">
+        <v>213</v>
       </c>
       <c r="G105">
         <v>0</v>
@@ -4234,8 +4564,11 @@
       <c r="H105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>106</v>
       </c>
@@ -4251,8 +4584,8 @@
       <c r="E106" t="s">
         <v>9</v>
       </c>
-      <c r="F106">
-        <v>0</v>
+      <c r="F106" t="s">
+        <v>213</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -4260,8 +4593,11 @@
       <c r="H106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>107</v>
       </c>
@@ -4277,8 +4613,8 @@
       <c r="E107" t="s">
         <v>9</v>
       </c>
-      <c r="F107">
-        <v>0</v>
+      <c r="F107" t="s">
+        <v>213</v>
       </c>
       <c r="G107">
         <v>0</v>
@@ -4286,8 +4622,11 @@
       <c r="H107">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>108</v>
       </c>
@@ -4303,8 +4642,8 @@
       <c r="E108" t="s">
         <v>9</v>
       </c>
-      <c r="F108">
-        <v>0</v>
+      <c r="F108" t="s">
+        <v>213</v>
       </c>
       <c r="G108">
         <v>0</v>
@@ -4312,8 +4651,11 @@
       <c r="H108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>109</v>
       </c>
@@ -4329,8 +4671,8 @@
       <c r="E109" t="s">
         <v>9</v>
       </c>
-      <c r="F109">
-        <v>0</v>
+      <c r="F109" t="s">
+        <v>213</v>
       </c>
       <c r="G109">
         <v>0</v>
@@ -4338,8 +4680,11 @@
       <c r="H109">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>110</v>
       </c>
@@ -4355,8 +4700,8 @@
       <c r="E110" t="s">
         <v>9</v>
       </c>
-      <c r="F110">
-        <v>0</v>
+      <c r="F110" t="s">
+        <v>213</v>
       </c>
       <c r="G110">
         <v>0</v>
@@ -4364,8 +4709,11 @@
       <c r="H110">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>111</v>
       </c>
@@ -4381,8 +4729,8 @@
       <c r="E111" t="s">
         <v>9</v>
       </c>
-      <c r="F111">
-        <v>0</v>
+      <c r="F111" t="s">
+        <v>213</v>
       </c>
       <c r="G111">
         <v>0</v>
@@ -4390,8 +4738,11 @@
       <c r="H111">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>112</v>
       </c>
@@ -4407,8 +4758,8 @@
       <c r="E112" t="s">
         <v>9</v>
       </c>
-      <c r="F112">
-        <v>0</v>
+      <c r="F112" t="s">
+        <v>213</v>
       </c>
       <c r="G112">
         <v>0</v>
@@ -4416,8 +4767,11 @@
       <c r="H112">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>113</v>
       </c>
@@ -4433,8 +4787,8 @@
       <c r="E113" t="s">
         <v>9</v>
       </c>
-      <c r="F113">
-        <v>0</v>
+      <c r="F113" t="s">
+        <v>213</v>
       </c>
       <c r="G113">
         <v>0</v>
@@ -4442,8 +4796,11 @@
       <c r="H113">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>114</v>
       </c>
@@ -4459,8 +4816,8 @@
       <c r="E114" t="s">
         <v>9</v>
       </c>
-      <c r="F114">
-        <v>0</v>
+      <c r="F114" t="s">
+        <v>213</v>
       </c>
       <c r="G114">
         <v>0</v>
@@ -4468,8 +4825,11 @@
       <c r="H114">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>115</v>
       </c>
@@ -4485,8 +4845,8 @@
       <c r="E115" t="s">
         <v>9</v>
       </c>
-      <c r="F115">
-        <v>0</v>
+      <c r="F115" t="s">
+        <v>213</v>
       </c>
       <c r="G115">
         <v>0</v>
@@ -4494,8 +4854,11 @@
       <c r="H115">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>116</v>
       </c>
@@ -4511,17 +4874,20 @@
       <c r="E116" t="s">
         <v>9</v>
       </c>
-      <c r="F116">
-        <v>0</v>
+      <c r="F116" t="s">
+        <v>211</v>
       </c>
       <c r="G116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>117</v>
       </c>
@@ -4537,17 +4903,20 @@
       <c r="E117" t="s">
         <v>9</v>
       </c>
-      <c r="F117">
-        <v>0</v>
+      <c r="F117" t="s">
+        <v>211</v>
       </c>
       <c r="G117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H117">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>118</v>
       </c>
@@ -4563,20 +4932,23 @@
       <c r="E118" t="s">
         <v>9</v>
       </c>
-      <c r="F118">
-        <v>0</v>
+      <c r="F118" t="s">
+        <v>211</v>
       </c>
       <c r="G118">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H118">
-        <v>0</v>
-      </c>
-      <c r="I118" t="s">
+        <v>1</v>
+      </c>
+      <c r="I118">
+        <v>0</v>
+      </c>
+      <c r="J118" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>119</v>
       </c>
@@ -4592,17 +4964,20 @@
       <c r="E119" t="s">
         <v>9</v>
       </c>
-      <c r="F119">
-        <v>0</v>
+      <c r="F119" t="s">
+        <v>211</v>
       </c>
       <c r="G119">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H119">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>120</v>
       </c>
@@ -4618,17 +4993,20 @@
       <c r="E120" t="s">
         <v>9</v>
       </c>
-      <c r="F120">
-        <v>0</v>
+      <c r="F120" t="s">
+        <v>211</v>
       </c>
       <c r="G120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H120">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>121</v>
       </c>
@@ -4644,17 +5022,20 @@
       <c r="E121" t="s">
         <v>9</v>
       </c>
-      <c r="F121">
-        <v>0</v>
+      <c r="F121" t="s">
+        <v>211</v>
       </c>
       <c r="G121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H121">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>122</v>
       </c>
@@ -4670,17 +5051,20 @@
       <c r="E122" t="s">
         <v>9</v>
       </c>
-      <c r="F122">
-        <v>0</v>
+      <c r="F122" t="s">
+        <v>211</v>
       </c>
       <c r="G122">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H122">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>123</v>
       </c>
@@ -4696,17 +5080,20 @@
       <c r="E123" t="s">
         <v>9</v>
       </c>
-      <c r="F123">
-        <v>0</v>
+      <c r="F123" t="s">
+        <v>211</v>
       </c>
       <c r="G123">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H123">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>124</v>
       </c>
@@ -4722,17 +5109,20 @@
       <c r="E124" t="s">
         <v>9</v>
       </c>
-      <c r="F124">
-        <v>0</v>
+      <c r="F124" t="s">
+        <v>211</v>
       </c>
       <c r="G124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H124">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>125</v>
       </c>
@@ -4748,17 +5138,20 @@
       <c r="E125" t="s">
         <v>9</v>
       </c>
-      <c r="F125">
-        <v>0</v>
+      <c r="F125" t="s">
+        <v>211</v>
       </c>
       <c r="G125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H125">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>126</v>
       </c>
@@ -4774,17 +5167,20 @@
       <c r="E126" t="s">
         <v>9</v>
       </c>
-      <c r="F126">
-        <v>0</v>
+      <c r="F126" t="s">
+        <v>211</v>
       </c>
       <c r="G126">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H126">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>127</v>
       </c>
@@ -4800,17 +5196,20 @@
       <c r="E127" t="s">
         <v>9</v>
       </c>
-      <c r="F127">
-        <v>0</v>
+      <c r="F127" t="s">
+        <v>211</v>
       </c>
       <c r="G127">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H127">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>128</v>
       </c>
@@ -4826,17 +5225,20 @@
       <c r="E128" t="s">
         <v>9</v>
       </c>
-      <c r="F128">
-        <v>0</v>
+      <c r="F128" t="s">
+        <v>211</v>
       </c>
       <c r="G128">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>129</v>
       </c>
@@ -4852,17 +5254,20 @@
       <c r="E129" t="s">
         <v>9</v>
       </c>
-      <c r="F129">
-        <v>0</v>
+      <c r="F129" t="s">
+        <v>211</v>
       </c>
       <c r="G129">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H129">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>130</v>
       </c>
@@ -4878,17 +5283,20 @@
       <c r="E130" t="s">
         <v>9</v>
       </c>
-      <c r="F130">
-        <v>0</v>
+      <c r="F130" t="s">
+        <v>211</v>
       </c>
       <c r="G130">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H130">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>131</v>
       </c>
@@ -4904,17 +5312,20 @@
       <c r="E131" t="s">
         <v>9</v>
       </c>
-      <c r="F131">
-        <v>0</v>
+      <c r="F131" t="s">
+        <v>211</v>
       </c>
       <c r="G131">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H131">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>132</v>
       </c>
@@ -4930,17 +5341,20 @@
       <c r="E132" t="s">
         <v>9</v>
       </c>
-      <c r="F132">
-        <v>0</v>
+      <c r="F132" t="s">
+        <v>211</v>
       </c>
       <c r="G132">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H132">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>133</v>
       </c>
@@ -4956,17 +5370,20 @@
       <c r="E133" t="s">
         <v>9</v>
       </c>
-      <c r="F133">
-        <v>0</v>
+      <c r="F133" t="s">
+        <v>211</v>
       </c>
       <c r="G133">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H133">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>134</v>
       </c>
@@ -4982,17 +5399,20 @@
       <c r="E134" t="s">
         <v>9</v>
       </c>
-      <c r="F134">
-        <v>0</v>
+      <c r="F134" t="s">
+        <v>211</v>
       </c>
       <c r="G134">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H134">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>135</v>
       </c>
@@ -5008,17 +5428,20 @@
       <c r="E135" t="s">
         <v>9</v>
       </c>
-      <c r="F135">
-        <v>0</v>
+      <c r="F135" t="s">
+        <v>211</v>
       </c>
       <c r="G135">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H135">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>136</v>
       </c>
@@ -5034,17 +5457,20 @@
       <c r="E136" t="s">
         <v>9</v>
       </c>
-      <c r="F136">
-        <v>0</v>
+      <c r="F136" t="s">
+        <v>211</v>
       </c>
       <c r="G136">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H136">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>137</v>
       </c>
@@ -5060,17 +5486,20 @@
       <c r="E137" t="s">
         <v>9</v>
       </c>
-      <c r="F137">
-        <v>0</v>
+      <c r="F137" t="s">
+        <v>211</v>
       </c>
       <c r="G137">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H137">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>138</v>
       </c>
@@ -5086,17 +5515,20 @@
       <c r="E138" t="s">
         <v>9</v>
       </c>
-      <c r="F138">
-        <v>0</v>
+      <c r="F138" t="s">
+        <v>211</v>
       </c>
       <c r="G138">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H138">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>139</v>
       </c>
@@ -5112,17 +5544,20 @@
       <c r="E139" t="s">
         <v>9</v>
       </c>
-      <c r="F139">
-        <v>0</v>
+      <c r="F139" t="s">
+        <v>211</v>
       </c>
       <c r="G139">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H139">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>140</v>
       </c>
@@ -5138,17 +5573,20 @@
       <c r="E140" t="s">
         <v>9</v>
       </c>
-      <c r="F140">
-        <v>0</v>
+      <c r="F140" t="s">
+        <v>211</v>
       </c>
       <c r="G140">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H140">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>141</v>
       </c>
@@ -5164,17 +5602,20 @@
       <c r="E141" t="s">
         <v>9</v>
       </c>
-      <c r="F141">
-        <v>0</v>
+      <c r="F141" t="s">
+        <v>211</v>
       </c>
       <c r="G141">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H141">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>142</v>
       </c>
@@ -5190,17 +5631,20 @@
       <c r="E142" t="s">
         <v>9</v>
       </c>
-      <c r="F142">
-        <v>0</v>
+      <c r="F142" t="s">
+        <v>211</v>
       </c>
       <c r="G142">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H142">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>143</v>
       </c>
@@ -5216,17 +5660,20 @@
       <c r="E143" t="s">
         <v>9</v>
       </c>
-      <c r="F143">
-        <v>0</v>
+      <c r="F143" t="s">
+        <v>211</v>
       </c>
       <c r="G143">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H143">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>144</v>
       </c>
@@ -5242,13 +5689,16 @@
       <c r="E144" t="s">
         <v>9</v>
       </c>
-      <c r="F144">
-        <v>0</v>
+      <c r="F144" t="s">
+        <v>212</v>
       </c>
       <c r="G144">
         <v>0</v>
       </c>
       <c r="H144">
+        <v>0</v>
+      </c>
+      <c r="I144">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
important, overrode long/lat from agouti with ones from CSV! Since on agouti we sometimes entered the wrong ones.
</commit_message>
<xml_diff>
--- a/coiba_camtrap_ids_gps.xlsx
+++ b/coiba_camtrap_ids_gps.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20400"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zoe Goldsborough\Documents\GitHub\camtrap_coiba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD679F8A-ECAC-4197-A65E-D78AD8AF40E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810E8677-3023-4032-A421-24C3E96394C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="221">
   <si>
     <t>number</t>
   </si>
@@ -671,6 +671,18 @@
   </si>
   <si>
     <t>northwest</t>
+  </si>
+  <si>
+    <t>7.270808333333333</t>
+  </si>
+  <si>
+    <t>-81.81914450833334</t>
+  </si>
+  <si>
+    <t>7.2704029</t>
+  </si>
+  <si>
+    <t>-81.8185249</t>
   </si>
 </sst>
 </file>
@@ -1515,8 +1527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="C138" sqref="C138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5361,11 +5373,11 @@
       <c r="B133" t="s">
         <v>142</v>
       </c>
-      <c r="C133" s="1">
-        <v>-81.819144508333295</v>
-      </c>
-      <c r="D133" s="1">
-        <v>7.2708083333333304</v>
+      <c r="C133" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="E133" t="s">
         <v>9</v>
@@ -5390,11 +5402,11 @@
       <c r="B134" t="s">
         <v>143</v>
       </c>
-      <c r="C134" s="1">
-        <v>-81.818473851308198</v>
-      </c>
-      <c r="D134" s="1">
-        <v>7.2703333105891899</v>
+      <c r="C134" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>219</v>
       </c>
       <c r="E134" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
took closer look at which long/lats didnt match. But need to still see how this affects co-occurrences so much!
</commit_message>
<xml_diff>
--- a/coiba_camtrap_ids_gps.xlsx
+++ b/coiba_camtrap_ids_gps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zoe Goldsborough\Documents\GitHub\camtrap_coiba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810E8677-3023-4032-A421-24C3E96394C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909399AA-1E44-4B39-984B-F7A09A396829}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="225">
   <si>
     <t>number</t>
   </si>
@@ -683,6 +683,18 @@
   </si>
   <si>
     <t>-81.8185249</t>
+  </si>
+  <si>
+    <t>7.2724829</t>
+  </si>
+  <si>
+    <t>-81.8218742</t>
+  </si>
+  <si>
+    <t>7.2705335</t>
+  </si>
+  <si>
+    <t>-81.8205352</t>
   </si>
 </sst>
 </file>
@@ -1527,8 +1539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="C138" sqref="C138"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3398,11 +3410,11 @@
       <c r="B65" t="s">
         <v>74</v>
       </c>
-      <c r="C65" s="1">
-        <v>-81.821971000000005</v>
-      </c>
-      <c r="D65" s="1">
-        <v>7.2731823000000002</v>
+      <c r="C65" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>221</v>
       </c>
       <c r="E65" t="s">
         <v>9</v>
@@ -3456,11 +3468,11 @@
       <c r="B67" t="s">
         <v>76</v>
       </c>
-      <c r="C67" s="1">
-        <v>-81.820188200000004</v>
-      </c>
-      <c r="D67" s="1">
-        <v>7.2714584999999996</v>
+      <c r="C67" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>223</v>
       </c>
       <c r="E67" t="s">
         <v>9</v>

</xml_diff>